<commit_message>
add multiple new feedstocks for TAL-KSA biorefineries
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_corn_Acrylic_300L_FGI.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/acrylic_acid_product/parameter-distributions_corn_Acrylic_300L_FGI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\acrylic_acid_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02890A86-F61C-47D5-9E37-0A0FC6364D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55D23D9-28B4-408E-8CAC-D5C76201AE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A18" sqref="A18:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1349,8 +1349,8 @@
         <v>22</v>
       </c>
       <c r="G18" s="4">
-        <f>E18*0.08</f>
-        <v>1.6240000000000001E-2</v>
+        <f>E18*0.8</f>
+        <v>0.16240000000000002</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4">
@@ -1362,7 +1362,7 @@
         <v>76</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" ref="Q18:Q19" si="3">IF(E18=H18, 1, IF(F18=$F$2, 1, 0))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1386,8 +1386,8 @@
         <v>22</v>
       </c>
       <c r="G19" s="4">
-        <f>E19*0.08</f>
-        <v>5.2800000000000004E-4</v>
+        <f>E19*0.8</f>
+        <v>5.28E-3</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4">
@@ -1399,7 +1399,7 @@
         <v>75</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1475,7 +1475,7 @@
         <v>54</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21" si="4">IF(E21=H21, 1, IF(F21=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q21" si="3">IF(E21=H21, 1, IF(F21=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
         <v>56</v>
       </c>
       <c r="Q26">
-        <f t="shared" ref="Q26:Q28" si="5">IF(E26=H26, 1, IF(F26=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q26:Q28" si="4">IF(E26=H26, 1, IF(F26=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
         <v>72</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
         <v>74</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
         <v>45</v>
       </c>
       <c r="Q30">
-        <f t="shared" ref="Q30:Q32" si="6">IF(E30=H30, 1, IF(F30=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q30:Q32" si="5">IF(E30=H30, 1, IF(F30=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
         <v>34</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -1878,7 +1878,7 @@
         <v>44</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>